<commit_message>
Pegar as frequencias das palavras e começar o smoothing
</commit_message>
<xml_diff>
--- a/iPhone.xlsx
+++ b/iPhone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/87e504f2267d2b3d/Ralph/Insper/2° semestre/Ciencia dos Dados/P1CDados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="114_{84B266C8-D8E9-4AEF-BBF4-1B62A16D542C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{62D94EF5-9156-4951-A01B-58FFF6AFA705}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="114_{84B266C8-D8E9-4AEF-BBF4-1B62A16D542C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1AE0A59-0EFC-4DED-9D7D-D902A5E271AE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2160,10 +2160,10 @@
     <t>@_ilipe quero um iphone 11 🤔</t>
   </si>
   <si>
-    <t xml:space="preserve">Classificação </t>
-  </si>
-  <si>
     <t>Relevância</t>
+  </si>
+  <si>
+    <t>Classificação</t>
   </si>
 </sst>
 </file>
@@ -2616,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView topLeftCell="A482" zoomScale="49" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21"/>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6648,7 +6648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
+    <sheetView zoomScale="55" workbookViewId="0">
       <selection activeCell="D240" sqref="D240"/>
     </sheetView>
   </sheetViews>
@@ -6663,7 +6663,7 @@
         <v>501</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>

</xml_diff>